<commit_message>
Se adicionó eltracker de Renewals cancelados
</commit_message>
<xml_diff>
--- a/Documents/Expected Critical Communications Report.xlsx
+++ b/Documents/Expected Critical Communications Report.xlsx
@@ -17346,7 +17346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="177">
+  <cellXfs count="178">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -17872,6 +17872,9 @@
     <xf numFmtId="0" fontId="176" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -18191,8 +18194,8 @@
   </sheetPr>
   <dimension ref="A1:N880"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -19120,7 +19123,7 @@
         <v>146</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="4" t="s">
+      <c r="F22" s="2" t="s">
         <v>147</v>
       </c>
       <c r="G22" s="46">
@@ -19138,7 +19141,7 @@
       <c r="K22" s="49" t="s">
         <v>148</v>
       </c>
-      <c r="L22" s="51" t="s">
+      <c r="L22" s="177" t="s">
         <v>75</v>
       </c>
       <c r="M22" s="32"/>

</xml_diff>

<commit_message>
simplificacion del critical communications
</commit_message>
<xml_diff>
--- a/Documents/Expected Critical Communications Report.xlsx
+++ b/Documents/Expected Critical Communications Report.xlsx
@@ -18195,7 +18195,7 @@
   <dimension ref="A1:N880"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18265,7 +18265,7 @@
       <c r="E2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
       <c r="G2" s="5">

</xml_diff>